<commit_message>
Calculate percentage of reads assigned FAPROTAX category
</commit_message>
<xml_diff>
--- a/data/cleaned/sequencing/faprotax-asv.xlsx
+++ b/data/cleaned/sequencing/faprotax-asv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/02_AVCA Elkhorn-Las Delicias/AVCA_ElkLD/data/cleaned/sequencing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{44E0D8B5-832F-4E48-9155-4E3BDF26D289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E95D09A-FA32-4ED6-8368-4E800E4916DB}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{44E0D8B5-832F-4E48-9155-4E3BDF26D289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{763B09EB-624E-461A-A634-21C0CB9D4AC6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{14C51EC9-9943-4685-9D79-B26A064BDD07}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{14C51EC9-9943-4685-9D79-B26A064BDD07}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -1820,11 +1820,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA11EA38-DBDA-4679-836E-028067EA33EB}">
   <dimension ref="A1:BI1941"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="135" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="141.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>